<commit_message>
#0 Clean up repo structure and notebooks
</commit_message>
<xml_diff>
--- a/paper/notebooks/datasets_plot/Plants datasets.xlsx
+++ b/paper/notebooks/datasets_plot/Plants datasets.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -388,7 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="220">
   <si>
     <t>name</t>
   </si>
@@ -639,7 +639,10 @@
     <t>location data can be null;</t>
   </si>
   <si>
-    <t>iNaturalist-300k</t>
+    <t>plantNaturalist-500k</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/datasets/anhaltai/plantNaturalist500k</t>
   </si>
   <si>
     <t>taxonomy</t>
@@ -1352,9 +1355,6 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -1362,6 +1362,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1628,8 +1631,9 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="30.0"/>
     <col customWidth="1" min="3" max="3" width="18.75"/>
+    <col customWidth="1" min="4" max="4" width="26.88"/>
     <col customWidth="1" min="9" max="9" width="16.88"/>
-    <col customWidth="1" min="16" max="16" width="16.13"/>
+    <col customWidth="1" min="16" max="16" width="85.38"/>
     <col customWidth="1" min="19" max="19" width="16.25"/>
     <col customWidth="1" min="29" max="29" width="38.25"/>
   </cols>
@@ -2386,7 +2390,9 @@
         <v>73</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="E10" s="3">
         <v>1.0</v>
       </c>
@@ -2397,23 +2403,23 @@
         <v>0.0</v>
       </c>
       <c r="H10" s="5">
-        <v>526584.0</v>
+        <v>500909.0</v>
       </c>
       <c r="I10" s="5" t="b">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J10" s="5">
-        <v>421294.0</v>
+        <v>300545.0</v>
       </c>
       <c r="K10" s="5">
-        <v>52726.0</v>
+        <v>100182.0</v>
       </c>
       <c r="L10" s="5">
-        <v>52564.0</v>
+        <v>100182.0</v>
       </c>
       <c r="M10" s="5">
-        <v>991.0</v>
+        <v>2490.0</v>
       </c>
       <c r="N10" s="5">
         <v>-1.0</v>
@@ -2422,7 +2428,7 @@
         <v>-1.0</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>35</v>
@@ -2430,7 +2436,7 @@
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="U10" s="3">
         <v>1.0</v>
@@ -2439,7 +2445,7 @@
         <v>38</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="X10" s="3">
         <v>1.0</v>
@@ -2457,21 +2463,21 @@
         <v>5.0</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E11" s="3">
         <v>1.0</v>
@@ -2509,13 +2515,13 @@
         <v>332864.0</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S11" s="3">
         <v>0.0</v>
@@ -2530,7 +2536,7 @@
         <v>38</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="X11" s="3">
         <v>0.0</v>
@@ -2548,19 +2554,19 @@
         <v>2.0</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E12" s="3">
         <v>1.0</v>
@@ -2598,13 +2604,13 @@
         <v>429145.0</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>35</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S12" s="3">
         <v>0.0</v>
@@ -2637,27 +2643,27 @@
         <v>1.0</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E13" s="3">
         <v>1.0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G13" s="3">
         <v>0.0</v>
@@ -2689,10 +2695,10 @@
         <v>-1.0</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>36</v>
@@ -2707,10 +2713,10 @@
         <v>0.0</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="X13" s="3">
         <v>0.0</v>
@@ -2728,27 +2734,27 @@
         <v>1.0</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E14" s="3">
         <v>1.0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G14" s="3">
         <v>0.0</v>
@@ -2780,10 +2786,10 @@
         <v>-1.0</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>36</v>
@@ -2796,10 +2802,10 @@
       </c>
       <c r="U14" s="6"/>
       <c r="V14" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="X14" s="3">
         <v>1.0</v>
@@ -2817,15 +2823,15 @@
         <v>0.0</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="3">
@@ -2857,7 +2863,7 @@
         <v>-1.0</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>35</v>
@@ -2886,19 +2892,19 @@
         <v>3.0</v>
       </c>
       <c r="AC15" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E16" s="3">
         <v>1.0</v>
@@ -2936,7 +2942,7 @@
         <v>-1.0</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>35</v>
@@ -2945,10 +2951,10 @@
         <v>36</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="U16" s="6"/>
       <c r="V16" s="3" t="s">
@@ -2973,21 +2979,21 @@
       <c r="AC16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>111</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E17" s="3">
         <v>1.0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G17" s="3">
         <v>1.0</v>
@@ -3026,10 +3032,10 @@
         <v>36</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U17" s="6"/>
       <c r="V17" s="3" t="s">
@@ -3052,22 +3058,22 @@
         <v>3.0</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AD17" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E18" s="3">
         <v>1.0</v>
@@ -3105,7 +3111,7 @@
         <v>-1.0</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q18" s="3" t="s">
         <v>35</v>
@@ -3114,10 +3120,10 @@
         <v>36</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U18" s="3">
         <v>1.0</v>
@@ -3142,28 +3148,28 @@
         <v>3.0</v>
       </c>
       <c r="AC18" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AD18" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>125</v>
+      <c r="A19" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E19" s="3">
         <v>1.0</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G19" s="3">
         <v>1.0</v>
@@ -3202,10 +3208,10 @@
         <v>36</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="3" t="s">
@@ -3228,28 +3234,28 @@
         <v>3.0</v>
       </c>
       <c r="AC19" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AD19" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" ht="18.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E20" s="3">
         <v>1.0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G20" s="3">
         <v>1.0</v>
@@ -3282,23 +3288,23 @@
         <v>-1.0</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>36</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="U20" s="6"/>
       <c r="V20" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W20" s="6"/>
       <c r="X20" s="3">
@@ -3320,25 +3326,25 @@
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E21" s="3">
         <v>0.0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G21" s="3">
         <v>1.0</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="12">
         <f t="shared" si="5"/>
         <v>330772</v>
       </c>
@@ -3346,13 +3352,13 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="12">
         <v>321270.0</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="12">
         <v>6316.0</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="12">
         <v>3186.0</v>
       </c>
       <c r="M21" s="5">
@@ -3365,25 +3371,25 @@
         <v>-1.0</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="U21" s="3">
         <v>1.0</v>
       </c>
       <c r="V21" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W21" s="6"/>
       <c r="X21" s="3">
@@ -3401,26 +3407,26 @@
       <c r="AB21" s="3">
         <v>2.0</v>
       </c>
-      <c r="AC21" s="14" t="s">
-        <v>140</v>
+      <c r="AC21" s="13" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E22" s="3">
         <v>0.0</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G22" s="3">
         <v>1.0</v>
@@ -3453,7 +3459,7 @@
         <v>-1.0</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>35</v>
@@ -3462,14 +3468,14 @@
         <v>36</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U22" s="6"/>
       <c r="V22" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W22" s="6"/>
       <c r="X22" s="3">
@@ -3488,25 +3494,25 @@
         <v>2.0</v>
       </c>
       <c r="AC22" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E23" s="3">
         <v>0.0</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G23" s="3">
         <v>1.0</v>
@@ -3539,7 +3545,7 @@
         <v>-1.0</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>35</v>
@@ -3548,14 +3554,14 @@
         <v>36</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="U23" s="6"/>
       <c r="V23" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="W23" s="6"/>
       <c r="X23" s="3">
@@ -3574,25 +3580,25 @@
         <v>2.0</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E24" s="3">
         <v>1.0</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G24" s="3">
         <v>0.0</v>
@@ -3618,7 +3624,7 @@
       </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R24" s="3" t="s">
         <v>36</v>
@@ -3629,7 +3635,7 @@
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
       <c r="V24" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W24" s="6"/>
       <c r="X24" s="3">
@@ -3648,25 +3654,25 @@
         <v>2.0</v>
       </c>
       <c r="AC24" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="3">
         <v>1.0</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G25" s="3">
         <v>0.0</v>
@@ -3690,7 +3696,7 @@
       </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R25" s="3" t="s">
         <v>36</v>
@@ -3701,7 +3707,7 @@
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="V25" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
@@ -3718,20 +3724,20 @@
         <v>1.0</v>
       </c>
       <c r="AC25" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="5">
@@ -3755,7 +3761,7 @@
       </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R26" s="3" t="s">
         <v>36</v>
@@ -3766,7 +3772,7 @@
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
       <c r="V26" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W26" s="6"/>
       <c r="X26" s="3">
@@ -3783,22 +3789,22 @@
         <v>1.0</v>
       </c>
       <c r="AC26" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="5">
@@ -3821,10 +3827,10 @@
         <v>-1.0</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R27" s="3" t="s">
         <v>36</v>
@@ -3835,7 +3841,7 @@
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
       <c r="V27" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W27" s="6"/>
       <c r="X27" s="3">
@@ -3852,22 +3858,22 @@
         <v>1.0</v>
       </c>
       <c r="AC27" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="3">
         <v>1.0</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="5">
@@ -3891,7 +3897,7 @@
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R28" s="3" t="s">
         <v>36</v>
@@ -3902,7 +3908,7 @@
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
       <c r="V28" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
@@ -3917,15 +3923,15 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="5">
@@ -3949,7 +3955,7 @@
       </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="R29" s="3" t="s">
         <v>36</v>
@@ -3960,7 +3966,7 @@
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
       <c r="V29" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W29" s="6"/>
       <c r="X29" s="3">
@@ -3977,23 +3983,23 @@
         <v>1.0</v>
       </c>
       <c r="AC29" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AD29" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="3">
@@ -4017,7 +4023,7 @@
       </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="R30" s="3" t="s">
         <v>36</v>
@@ -4037,23 +4043,23 @@
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
       <c r="AC30" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AD30" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="3">
@@ -4077,7 +4083,7 @@
       </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="R31" s="3" t="s">
         <v>36</v>
@@ -4096,24 +4102,24 @@
       </c>
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
-      <c r="AC31" s="11" t="s">
-        <v>172</v>
+      <c r="AC31" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="AD31" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="3">
@@ -4137,7 +4143,7 @@
       </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>36</v>
@@ -4146,7 +4152,7 @@
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
       <c r="V32" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W32" s="6"/>
       <c r="X32" s="6"/>
@@ -4158,24 +4164,24 @@
       </c>
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
-      <c r="AC32" s="11" t="s">
-        <v>174</v>
+      <c r="AC32" s="14" t="s">
+        <v>175</v>
       </c>
       <c r="AD32" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="3">
@@ -4199,7 +4205,7 @@
       </c>
       <c r="P33" s="6"/>
       <c r="Q33" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="R33" s="3" t="s">
         <v>36</v>
@@ -4208,7 +4214,7 @@
       <c r="T33" s="6"/>
       <c r="U33" s="6"/>
       <c r="V33" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W33" s="6"/>
       <c r="X33" s="6"/>
@@ -4220,24 +4226,24 @@
       </c>
       <c r="AA33" s="6"/>
       <c r="AB33" s="6"/>
-      <c r="AC33" s="11" t="s">
-        <v>176</v>
+      <c r="AC33" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="AD33" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="3">
@@ -4261,7 +4267,7 @@
       </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>36</v>
@@ -4270,7 +4276,7 @@
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
       <c r="V34" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W34" s="6"/>
       <c r="X34" s="6"/>
@@ -4282,24 +4288,24 @@
       </c>
       <c r="AA34" s="6"/>
       <c r="AB34" s="6"/>
-      <c r="AC34" s="11" t="s">
-        <v>178</v>
+      <c r="AC34" s="14" t="s">
+        <v>179</v>
       </c>
       <c r="AD34" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="3">
@@ -4323,7 +4329,7 @@
       </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="R35" s="3" t="s">
         <v>36</v>
@@ -4332,7 +4338,7 @@
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
       <c r="V35" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W35" s="6"/>
       <c r="X35" s="6"/>
@@ -4345,30 +4351,30 @@
       <c r="AA35" s="6"/>
       <c r="AB35" s="6"/>
       <c r="AC35" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AD35" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E36" s="3">
         <v>1.0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G36" s="3">
         <v>1.0</v>
@@ -4380,13 +4386,13 @@
         <f>SUM(J36,L36,K36)=H36</f>
         <v>1</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="13">
         <v>2257759.0</v>
       </c>
       <c r="K36" s="3">
         <v>0.0</v>
       </c>
-      <c r="L36" s="14">
+      <c r="L36" s="13">
         <v>243020.0</v>
       </c>
       <c r="M36" s="3">
@@ -4399,10 +4405,10 @@
         <v>-1.0</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="R36" s="3" t="s">
         <v>36</v>
@@ -4411,16 +4417,16 @@
         <v>0.0</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="U36" s="3">
         <v>1.0</v>
       </c>
       <c r="V36" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W36" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="X36" s="3">
         <v>1.0</v>
@@ -4437,8 +4443,8 @@
       <c r="AB36" s="3">
         <v>3.0</v>
       </c>
-      <c r="AC36" s="11" t="s">
-        <v>186</v>
+      <c r="AC36" s="14" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="50">
@@ -4473,34 +4479,35 @@
     <hyperlink r:id="rId11" ref="D7"/>
     <hyperlink r:id="rId12" ref="D8"/>
     <hyperlink r:id="rId13" ref="D9"/>
-    <hyperlink r:id="rId14" ref="C11"/>
-    <hyperlink r:id="rId15" ref="D11"/>
-    <hyperlink r:id="rId16" ref="D12"/>
-    <hyperlink r:id="rId17" ref="C13"/>
-    <hyperlink r:id="rId18" ref="D13"/>
-    <hyperlink r:id="rId19" ref="AC13"/>
-    <hyperlink r:id="rId20" ref="C14"/>
-    <hyperlink r:id="rId21" ref="D14"/>
-    <hyperlink r:id="rId22" ref="AC15"/>
-    <hyperlink r:id="rId23" ref="D16"/>
-    <hyperlink r:id="rId24" ref="D17"/>
-    <hyperlink r:id="rId25" ref="D18"/>
-    <hyperlink r:id="rId26" ref="D19"/>
-    <hyperlink r:id="rId27" ref="D20"/>
-    <hyperlink r:id="rId28" ref="D21"/>
-    <hyperlink r:id="rId29" ref="D22"/>
-    <hyperlink r:id="rId30" ref="D23"/>
-    <hyperlink r:id="rId31" ref="D24"/>
-    <hyperlink r:id="rId32" ref="C25"/>
-    <hyperlink r:id="rId33" ref="D27"/>
-    <hyperlink r:id="rId34" ref="AC29"/>
-    <hyperlink r:id="rId35" ref="AC30"/>
-    <hyperlink r:id="rId36" ref="AC35"/>
-    <hyperlink r:id="rId37" ref="C36"/>
-    <hyperlink r:id="rId38" ref="D36"/>
+    <hyperlink r:id="rId14" ref="D10"/>
+    <hyperlink r:id="rId15" ref="C11"/>
+    <hyperlink r:id="rId16" ref="D11"/>
+    <hyperlink r:id="rId17" ref="D12"/>
+    <hyperlink r:id="rId18" ref="C13"/>
+    <hyperlink r:id="rId19" ref="D13"/>
+    <hyperlink r:id="rId20" ref="AC13"/>
+    <hyperlink r:id="rId21" ref="C14"/>
+    <hyperlink r:id="rId22" ref="D14"/>
+    <hyperlink r:id="rId23" ref="AC15"/>
+    <hyperlink r:id="rId24" ref="D16"/>
+    <hyperlink r:id="rId25" ref="D17"/>
+    <hyperlink r:id="rId26" ref="D18"/>
+    <hyperlink r:id="rId27" ref="D19"/>
+    <hyperlink r:id="rId28" ref="D20"/>
+    <hyperlink r:id="rId29" ref="D21"/>
+    <hyperlink r:id="rId30" ref="D22"/>
+    <hyperlink r:id="rId31" ref="D23"/>
+    <hyperlink r:id="rId32" ref="D24"/>
+    <hyperlink r:id="rId33" ref="C25"/>
+    <hyperlink r:id="rId34" ref="D27"/>
+    <hyperlink r:id="rId35" ref="AC29"/>
+    <hyperlink r:id="rId36" ref="AC30"/>
+    <hyperlink r:id="rId37" ref="AC35"/>
+    <hyperlink r:id="rId38" ref="C36"/>
+    <hyperlink r:id="rId39" ref="D36"/>
   </hyperlinks>
-  <drawing r:id="rId39"/>
-  <legacyDrawing r:id="rId40"/>
+  <drawing r:id="rId40"/>
+  <legacyDrawing r:id="rId41"/>
 </worksheet>
 </file>
 
@@ -4519,16 +4526,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
@@ -4554,63 +4561,63 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -4727,7 +4734,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D2" s="3">
         <v>1.0</v>
@@ -4790,7 +4797,7 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>41</v>
@@ -4820,7 +4827,7 @@
         <v>-1.0</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>35</v>
@@ -4904,7 +4911,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D5" s="3">
         <v>1.0</v>
@@ -5105,7 +5112,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D8" s="3">
         <v>1.0</v>
@@ -5172,13 +5179,13 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D9" s="3">
         <v>1.0</v>
@@ -5202,13 +5209,13 @@
         <v>332864.0</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N9" s="3">
         <v>0.0</v>
@@ -5223,7 +5230,7 @@
         <v>38</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S9" s="3">
         <v>0.0</v>
@@ -5238,16 +5245,16 @@
         <v>2.0</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D10" s="3">
         <v>1.0</v>
@@ -5271,13 +5278,13 @@
         <v>429145.0</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N10" s="3">
         <v>0.0</v>
@@ -5307,24 +5314,24 @@
         <v>1.0</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D11" s="3">
         <v>1.0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F11" s="3">
         <v>0.0</v>
@@ -5342,10 +5349,10 @@
         <v>-1.0</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>36</v>
@@ -5360,10 +5367,10 @@
         <v>0.0</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="S11" s="3">
         <v>0.0</v>
@@ -5378,24 +5385,24 @@
         <v>1.0</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D12" s="3">
         <v>1.0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F12" s="3">
         <v>0.0</v>
@@ -5413,10 +5420,10 @@
         <v>-1.0</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>36</v>
@@ -5429,10 +5436,10 @@
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="S12" s="3">
         <v>1.0</v>
@@ -5447,12 +5454,12 @@
         <v>0.0</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="3">
@@ -5501,27 +5508,27 @@
         <v>3.0</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D14" s="3">
         <v>0.0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F14" s="3">
         <v>1.0</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <f>321270+6316+3186</f>
         <v>330772</v>
       </c>
@@ -5535,25 +5542,25 @@
         <v>-1.0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="P14" s="3">
         <v>1.0</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="3">
@@ -5568,23 +5575,23 @@
       <c r="V14" s="3">
         <v>2.0</v>
       </c>
-      <c r="W14" s="14" t="s">
-        <v>140</v>
+      <c r="W14" s="13" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="15" ht="18.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D15" s="3">
         <v>1.0</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F15" s="3">
         <v>1.0</v>
@@ -5603,23 +5610,23 @@
         <v>-1.0</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>36</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="3">
@@ -5638,17 +5645,17 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D16" s="3">
         <v>0.0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F16" s="3">
         <v>1.0</v>
@@ -5667,7 +5674,7 @@
         <v>-1.0</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>35</v>
@@ -5676,14 +5683,14 @@
         <v>36</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="3">
@@ -5699,22 +5706,22 @@
         <v>2.0</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D17" s="3">
         <v>0.0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F17" s="3">
         <v>1.0</v>
@@ -5733,7 +5740,7 @@
         <v>-1.0</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>35</v>
@@ -5742,14 +5749,14 @@
         <v>36</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R17" s="6"/>
       <c r="S17" s="3">
@@ -5765,16 +5772,16 @@
         <v>2.0</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D18" s="3">
         <v>1.0</v>
@@ -5799,7 +5806,7 @@
         <v>-1.0</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>35</v>
@@ -5808,10 +5815,10 @@
         <v>36</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="3" t="s">
@@ -5833,18 +5840,18 @@
       <c r="W18" s="6"/>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="s">
-        <v>110</v>
+      <c r="A19" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D19" s="3">
         <v>1.0</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F19" s="3">
         <v>1.0</v>
@@ -5870,10 +5877,10 @@
         <v>36</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="3" t="s">
@@ -5893,25 +5900,25 @@
         <v>3.0</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="X19" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="12" t="s">
-        <v>125</v>
+      <c r="A20" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D20" s="3">
         <v>1.0</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F20" s="3">
         <v>1.0</v>
@@ -5937,10 +5944,10 @@
         <v>36</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="3" t="s">
@@ -5960,19 +5967,19 @@
         <v>3.0</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="X20" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D21" s="3">
         <v>1.0</v>
@@ -5997,7 +6004,7 @@
         <v>-1.0</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>35</v>
@@ -6006,10 +6013,10 @@
         <v>36</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="P21" s="3">
         <v>1.0</v>
@@ -6031,25 +6038,25 @@
         <v>3.0</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="X21" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D22" s="3">
         <v>1.0</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F22" s="3">
         <v>0.0</v>
@@ -6068,7 +6075,7 @@
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>36</v>
@@ -6079,7 +6086,7 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R22" s="6"/>
       <c r="S22" s="3">
@@ -6095,22 +6102,22 @@
         <v>2.0</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="3">
         <v>1.0</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F23" s="3">
         <v>0.0</v>
@@ -6127,7 +6134,7 @@
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>36</v>
@@ -6138,7 +6145,7 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
@@ -6152,17 +6159,17 @@
         <v>1.0</v>
       </c>
       <c r="W23" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="5">
@@ -6179,7 +6186,7 @@
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>36</v>
@@ -6190,7 +6197,7 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R24" s="6"/>
       <c r="S24" s="3">
@@ -6204,19 +6211,19 @@
         <v>1.0</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5">
@@ -6232,10 +6239,10 @@
         <v>-1.0</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>36</v>
@@ -6246,7 +6253,7 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R25" s="6"/>
       <c r="S25" s="3">
@@ -6260,19 +6267,19 @@
         <v>1.0</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="3">
         <v>1.0</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="5">
@@ -6289,7 +6296,7 @@
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>36</v>
@@ -6300,7 +6307,7 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
@@ -6312,12 +6319,12 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="5">
@@ -6334,7 +6341,7 @@
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>36</v>
@@ -6345,7 +6352,7 @@
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R27" s="6"/>
       <c r="S27" s="3">
@@ -6359,20 +6366,20 @@
         <v>1.0</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="X27" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="3">
@@ -6389,7 +6396,7 @@
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>36</v>
@@ -6406,20 +6413,20 @@
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
       <c r="W28" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="X28" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="3">
@@ -6436,7 +6443,7 @@
       </c>
       <c r="K29" s="6"/>
       <c r="L29" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>36</v>
@@ -6452,21 +6459,21 @@
       </c>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
-      <c r="W29" s="11" t="s">
-        <v>172</v>
+      <c r="W29" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="X29" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="3">
@@ -6483,7 +6490,7 @@
       </c>
       <c r="K30" s="6"/>
       <c r="L30" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>36</v>
@@ -6492,7 +6499,7 @@
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R30" s="6"/>
       <c r="S30" s="6"/>
@@ -6501,21 +6508,21 @@
       </c>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
-      <c r="W30" s="11" t="s">
-        <v>174</v>
+      <c r="W30" s="14" t="s">
+        <v>175</v>
       </c>
       <c r="X30" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="3">
@@ -6532,7 +6539,7 @@
       </c>
       <c r="K31" s="6"/>
       <c r="L31" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>36</v>
@@ -6541,7 +6548,7 @@
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R31" s="6"/>
       <c r="S31" s="6"/>
@@ -6550,21 +6557,21 @@
       </c>
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
-      <c r="W31" s="11" t="s">
-        <v>176</v>
+      <c r="W31" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="X31" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="3">
@@ -6581,7 +6588,7 @@
       </c>
       <c r="K32" s="6"/>
       <c r="L32" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M32" s="3" t="s">
         <v>36</v>
@@ -6590,7 +6597,7 @@
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R32" s="6"/>
       <c r="S32" s="6"/>
@@ -6599,21 +6606,21 @@
       </c>
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
-      <c r="W32" s="11" t="s">
-        <v>178</v>
+      <c r="W32" s="14" t="s">
+        <v>179</v>
       </c>
       <c r="X32" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="3">
@@ -6630,7 +6637,7 @@
       </c>
       <c r="K33" s="6"/>
       <c r="L33" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M33" s="3" t="s">
         <v>36</v>
@@ -6639,7 +6646,7 @@
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R33" s="6"/>
       <c r="S33" s="6"/>
@@ -6649,27 +6656,27 @@
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
       <c r="W33" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="X33" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D34" s="3">
         <v>1.0</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F34" s="3">
         <v>1.0</v>
@@ -6688,7 +6695,7 @@
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="M34" s="3" t="s">
         <v>36</v>
@@ -6697,16 +6704,16 @@
         <v>0.0</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="P34" s="3">
         <v>1.0</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R34" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="S34" s="3">
         <v>1.0</v>
@@ -6720,11 +6727,11 @@
       <c r="V34" s="3">
         <v>3.0</v>
       </c>
-      <c r="W34" s="11" t="s">
-        <v>186</v>
+      <c r="W34" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>